<commit_message>
Oppdaterte resultatfiler. Lagt med rådata fra pocket query i gpx-filer
</commit_message>
<xml_diff>
--- a/X-Helg 2016 Statistikk.xlsx
+++ b/X-Helg 2016 Statistikk.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="101">
   <si>
     <t>Nick</t>
   </si>
@@ -162,9 +162,6 @@
     <t>13</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>8</t>
   </si>
   <si>
@@ -249,12 +246,6 @@
     <t>[#2] [#4] [#5] [#9]  (8)</t>
   </si>
   <si>
-    <t>[#4] [#5]  (4)</t>
-  </si>
-  <si>
-    <t>[#2] [#9] [#10]  (3)</t>
-  </si>
-  <si>
     <t>[#4] [#5] [#6] [#9]  (8)</t>
   </si>
   <si>
@@ -309,50 +300,56 @@
     <t>[#2] [#6] [#3]  (3)</t>
   </si>
   <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Brustadteam</t>
+  </si>
+  <si>
+    <t>[#11]  (2)</t>
+  </si>
+  <si>
+    <t>X-Helg 2016</t>
+  </si>
+  <si>
+    <t>[#12]  (3)</t>
+  </si>
+  <si>
+    <t>109 logger totalt i Desember!</t>
+  </si>
+  <si>
+    <t>FTF gir 3p, 2p for co-FTF</t>
+  </si>
+  <si>
+    <t>Publisert selv</t>
+  </si>
+  <si>
+    <t>Funn på publ dato</t>
+  </si>
+  <si>
+    <t>Funn i Desember</t>
+  </si>
+  <si>
+    <t>[#4] [#5] [#10]  (6)</t>
+  </si>
+  <si>
+    <t>[#2] [#9]  (2)</t>
+  </si>
+  <si>
     <t>[#9] [#6]  (6)</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Brustadteam</t>
-  </si>
-  <si>
-    <t>[#11]  (2)</t>
-  </si>
-  <si>
-    <t>Sist oppdatert</t>
-  </si>
-  <si>
-    <t>X-Helg 2016</t>
-  </si>
-  <si>
-    <t>[#12]  (3)</t>
-  </si>
-  <si>
-    <t>12/12/2016 kl 21.13</t>
-  </si>
-  <si>
-    <t>109 logger totalt i Desember!</t>
-  </si>
-  <si>
-    <t>Publisert selv (3p)</t>
-  </si>
-  <si>
-    <t>FTF gir 3p, 2p for co-FTF</t>
-  </si>
-  <si>
-    <t>Funn på publ dato (2p)</t>
-  </si>
-  <si>
-    <t>Funn i Desember (1p)</t>
+    <t>12/12/2016 kl 22.17</t>
+  </si>
+  <si>
+    <t>Sist oppdatert:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -496,6 +493,13 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -872,7 +876,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="22" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -881,6 +884,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - uthevingsfarge 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1243,53 +1249,53 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="33" style="3" customWidth="1"/>
+    <col min="5" max="5" width="25" style="3" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="C2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="F2" s="9" t="s">
+      <c r="E2" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1298,13 +1304,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="1" t="s">
@@ -1318,7 +1324,7 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="1" t="s">
@@ -1330,16 +1336,16 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>6</v>
@@ -1350,16 +1356,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>8</v>
@@ -1370,16 +1376,16 @@
         <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>8</v>
@@ -1390,16 +1396,16 @@
         <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>8</v>
@@ -1411,16 +1417,16 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1429,14 +1435,14 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1446,10 +1452,10 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>39</v>
@@ -1460,11 +1466,11 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="1" t="s">
@@ -1477,16 +1483,16 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1496,13 +1502,13 @@
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
       <c r="D14" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1510,17 +1516,17 @@
         <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1528,15 +1534,15 @@
         <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1544,15 +1550,15 @@
         <v>18</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1562,7 +1568,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
       <c r="D18" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="1" t="s">
@@ -1576,10 +1582,10 @@
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
       <c r="D19" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>23</v>
@@ -1590,7 +1596,7 @@
         <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="4"/>
@@ -1604,7 +1610,7 @@
         <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="4"/>
@@ -1615,10 +1621,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="4"/>
@@ -1635,7 +1641,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>32</v>
@@ -1643,12 +1649,12 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
       <c r="D24" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="1" t="s">
@@ -1662,7 +1668,7 @@
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="1" t="s">
@@ -1676,7 +1682,7 @@
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="1" t="s">
@@ -1690,7 +1696,7 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="1" t="s">
@@ -1704,7 +1710,7 @@
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="1" t="s">
@@ -1719,7 +1725,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>32</v>
@@ -1733,7 +1739,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>35</v>
@@ -1747,7 +1753,7 @@
       <c r="C31" s="1"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
New version of PS script. Now filters on log type. Only "Attended" (for events) and "Found it" counts in the stats.
</commit_message>
<xml_diff>
--- a/X-Helg 2016 Statistikk.xlsx
+++ b/X-Helg 2016 Statistikk.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Ark1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$2:$F$31</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$F$33</definedName>
+    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$2:$F$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$F$35</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="108">
   <si>
     <t>Nick</t>
   </si>
@@ -153,9 +153,6 @@
     <t>mirg75</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
     <t>18</t>
   </si>
   <si>
@@ -177,12 +174,6 @@
     <t>[#2]*  (2)</t>
   </si>
   <si>
-    <t>[#1] [#2] [#3] [#4] [#5] [#6] [#9] [#10]  (16)</t>
-  </si>
-  <si>
-    <t>[#1] [#2] [#3] [#4] [#5] [#6] [#7] [#9] [#10]  (18)</t>
-  </si>
-  <si>
     <t>[#6]  (3)</t>
   </si>
   <si>
@@ -213,33 +204,21 @@
     <t>[#1] [#3]  (6)</t>
   </si>
   <si>
-    <t>[#10]  (2)</t>
-  </si>
-  <si>
     <t>[#1] [#2] [#3] [#4] [#5]  (5)</t>
   </si>
   <si>
     <t>[#2]* [#4]  (5)</t>
   </si>
   <si>
-    <t>[#2] [#4]  (4)</t>
-  </si>
-  <si>
     <t>[#1] [#3] [#5] [#6] [#9] [#10]  (6)</t>
   </si>
   <si>
     <t>15</t>
   </si>
   <si>
-    <t>[#2] [#4] [#5] [#9] [#10]  (10)</t>
-  </si>
-  <si>
     <t>[#1] [#3] [#6]  (3)</t>
   </si>
   <si>
-    <t>[#5] [#7] [#9] [#10]  (8)</t>
-  </si>
-  <si>
     <t>[#1]  (3)</t>
   </si>
   <si>
@@ -267,9 +246,6 @@
     <t>[#1] [#2]  (4)</t>
   </si>
   <si>
-    <t>[#9]  (2)</t>
-  </si>
-  <si>
     <t>[#3]  (3)</t>
   </si>
   <si>
@@ -315,9 +291,6 @@
     <t>[#12]  (3)</t>
   </si>
   <si>
-    <t>109 logger totalt i Desember!</t>
-  </si>
-  <si>
     <t>FTF gir 3p, 2p for co-FTF</t>
   </si>
   <si>
@@ -330,19 +303,67 @@
     <t>Funn i Desember</t>
   </si>
   <si>
-    <t>[#4] [#5] [#10]  (6)</t>
-  </si>
-  <si>
     <t>[#2] [#9]  (2)</t>
   </si>
   <si>
     <t>[#9] [#6]  (6)</t>
   </si>
   <si>
-    <t>12/12/2016 kl 22.17</t>
-  </si>
-  <si>
     <t>Sist oppdatert:</t>
+  </si>
+  <si>
+    <t>[#1] [#2] [#3] [#4] [#5] [#6] [#7] [#9] [#10] [#12] [#13]  (22)</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>[#1] [#2] [#3] [#5] [#6] [#9] [#10]  (14)</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>[#10] [#13]  (4)</t>
+  </si>
+  <si>
+    <t>[#2] [#4] [#13]  (6)</t>
+  </si>
+  <si>
+    <t>[#5] [#9] [#10] [#13]  (8)</t>
+  </si>
+  <si>
+    <t>[#2] [#4] [#5] [#9] [#10] [#13]  (12)</t>
+  </si>
+  <si>
+    <t>[#4] [#5] [#10] [#13]  (8)</t>
+  </si>
+  <si>
+    <t>[#13]  (3)</t>
+  </si>
+  <si>
+    <t>[#6] [#2] [#10]  (3)</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>[#9] [#13]  (4)</t>
+  </si>
+  <si>
+    <t>[#13]  (2)</t>
+  </si>
+  <si>
+    <t>Cachenissen</t>
+  </si>
+  <si>
+    <t>Hogg1</t>
+  </si>
+  <si>
+    <t>139 logger hittil i Desember!</t>
+  </si>
+  <si>
+    <t>13/12/2016 kl 21.55</t>
   </si>
 </sst>
 </file>
@@ -1246,7 +1267,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -1257,26 +1278,26 @@
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33" style="3" customWidth="1"/>
+    <col min="4" max="4" width="32" style="3" customWidth="1"/>
     <col min="5" max="5" width="25" style="3" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -1284,16 +1305,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>2</v>
@@ -1301,214 +1322,218 @@
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>43</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D4" s="4" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="1" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="C9" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="C10" s="1"/>
       <c r="D10" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="4"/>
+        <v>97</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="F10" s="1" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="D11" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>64</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="E11" s="4"/>
       <c r="F11" s="1" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="D12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="4"/>
+        <v>98</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="F12" s="1" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="1"/>
       <c r="D13" s="4" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>15</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>54</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E14" s="4"/>
       <c r="F14" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1516,101 +1541,103 @@
         <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="4" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>90</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B16" s="1"/>
       <c r="C16" s="2"/>
       <c r="D16" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="4"/>
+        <v>102</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="F16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="C18" s="2"/>
       <c r="D18" s="4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="1" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
       <c r="D19" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>50</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="E19" s="4"/>
       <c r="F19" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>76</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B20" s="1"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="D20" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="F20" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="4"/>
@@ -1621,10 +1648,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="4"/>
@@ -1635,35 +1662,35 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="4" t="s">
-        <v>79</v>
-      </c>
+      <c r="E23" s="4"/>
       <c r="F23" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F24" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1677,12 +1704,12 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="4" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="1" t="s">
@@ -1691,12 +1718,12 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="1" t="s">
@@ -1705,12 +1732,12 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="1" t="s">
@@ -1719,48 +1746,76 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4" t="s">
-        <v>81</v>
-      </c>
+      <c r="D29" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E29" s="4"/>
       <c r="F29" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="D30" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="4"/>
       <c r="F30" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4" t="s">
-        <v>82</v>
-      </c>
+      <c r="D31" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="4"/>
       <c r="F31" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>35</v>
       </c>
     </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lagt til ranking-funksjon i statistikken.
</commit_message>
<xml_diff>
--- a/X-Helg 2016 Statistikk.xlsx
+++ b/X-Helg 2016 Statistikk.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Ark1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$2:$F$36</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$F$38</definedName>
+    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$3:$G$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$G$40</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="123">
   <si>
     <t>Nick</t>
   </si>
@@ -270,9 +270,6 @@
     <t>Hogg1</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
     <t>[#1] [#4] [#5] [#9] [#10] [#13]  (12)</t>
   </si>
   <si>
@@ -354,27 +351,18 @@
     <t>[#16]  (3)</t>
   </si>
   <si>
-    <t>28</t>
-  </si>
-  <si>
     <t>[#16]* [#1] [#3]  (8)</t>
   </si>
   <si>
     <t>[#2] [#16]  (2)</t>
   </si>
   <si>
-    <t>27</t>
-  </si>
-  <si>
     <t>[#1] [#4] [#5] [#6] [#9] [#14] [#15] [#16]  (16)</t>
   </si>
   <si>
     <t>[#2] [#3] [#15]  (3)</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>[#16]* [#5]  (5)</t>
   </si>
   <si>
@@ -384,15 +372,9 @@
     <t>[#1] [#2] [#3] [#4] [#5] [#6] [#7] [#9] [#10] [#12] [#13] [#14] [#15] [#16]  (28)</t>
   </si>
   <si>
-    <t>31</t>
-  </si>
-  <si>
     <t>[#1] [#2] [#4] [#5] [#9] [#10] [#13] [#14] [#15] [#16]  (20)</t>
   </si>
   <si>
-    <t>22</t>
-  </si>
-  <si>
     <t>[#10]  (1)</t>
   </si>
   <si>
@@ -406,6 +388,27 @@
   </si>
   <si>
     <t>145 besøk logget hittil i Desember!</t>
+  </si>
+  <si>
+    <t>Plass</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>18</t>
   </si>
 </sst>
 </file>
@@ -554,15 +557,15 @@
       <family val="4"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -750,7 +753,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -880,6 +883,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -925,30 +937,37 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="22" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1309,614 +1328,727 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="37" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E1" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="11">
+      <c r="F1" s="7">
         <f ca="1">NOW()</f>
-        <v>42721.927336689812</v>
-      </c>
-      <c r="C1" s="7" t="s">
+        <v>42721.960884722219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D2" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" s="8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G16" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G23" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="B24" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G36" s="8">
         <v>1</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E6" s="4" t="s">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E34" s="4"/>
-      <c r="F34" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>34</v>
+      <c r="G37" s="8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="75" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="70" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>